<commit_message>
Support File Input Data
</commit_message>
<xml_diff>
--- a/static/files/DateListNotibalityAnalyse.xlsx
+++ b/static/files/DateListNotibalityAnalyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeHiu\Desktop\Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C0372-DE27-49E1-8B60-378A78804A2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4818614-9C88-4EC5-9812-637FAF58EB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28695" yWindow="960" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,7 +59,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Trun</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>基金</t>
+  </si>
+  <si>
+    <t>Foolish</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Turn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Balance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,10 +130,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -242,144 +275,129 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44565</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>44572</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>44573</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>44573</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44574</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>44575</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>44576</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>44577</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>44578</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>44579</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>44580</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>44581</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>44583</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>44584</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>44585</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44586</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44587</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44588</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>44589</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>44590</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44591</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44592</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44593</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44594</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44596</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44597</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44598</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44599</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44600</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44601</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44602</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44603</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44604</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44606</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$B$2:$B$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00_);[Red]\(0.00\)">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7" formatCode="0.00_);[Red]\(0.00\)">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>7.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -431,144 +449,126 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44565</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>44572</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>44573</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>44573</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44574</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>44575</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>44576</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>44577</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>44578</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>44579</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>44580</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>44581</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>44583</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>44584</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>44585</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44586</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44587</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44588</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>44589</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>44590</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44591</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44592</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44593</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44594</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44596</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44597</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44598</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44599</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44600</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44601</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44602</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44603</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44604</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44606</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$37</c:f>
+              <c:f>Sheet1!$C$2:$C$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,144 +620,126 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44565</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>44572</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>44573</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>44573</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44574</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>44575</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>44576</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>44577</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>44578</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>44579</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>44580</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>44581</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>44583</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="16">
                   <c:v>44584</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>44585</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44586</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44587</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44588</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>44589</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>44590</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44591</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44592</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44593</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44594</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44596</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44597</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44598</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44599</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44600</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44601</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44602</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44603</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44604</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44606</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44607</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$37</c:f>
+              <c:f>Sheet1!$D$2:$D$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7" formatCode="0.00_);[Red]\(0.00\)">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10" formatCode="0.00_);[Red]\(0.00\)">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,7 +835,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00_);[Red]\(0.00\)" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1515,16 +1497,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1815,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1848,253 +1830,318 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>44572</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B2" s="3">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>44573</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="4">
+        <v>44563</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>44574</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="4">
+        <v>44564</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>44575</v>
-      </c>
-      <c r="B5" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="A5" s="4">
+        <v>44565</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44576</v>
+        <v>44572</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44577</v>
+        <v>44573</v>
       </c>
       <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
       <c r="D7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>44578</v>
-      </c>
+      <c r="A8" s="4">
+        <v>44573</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44579</v>
+        <v>44574</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44580</v>
+        <v>44575</v>
+      </c>
+      <c r="B10" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44581</v>
+        <v>44576</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44582</v>
+        <v>44577</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>44583</v>
+      <c r="A13" s="4">
+        <v>44578</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>44584</v>
+      <c r="A14" s="4">
+        <v>44579</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>44585</v>
+      <c r="A15" s="4">
+        <v>44580</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>44586</v>
+      <c r="A16" s="4">
+        <v>44581</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>44587</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>44583</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>44588</v>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>44584</v>
+      </c>
+      <c r="B18" s="3">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>44589</v>
+        <v>44590</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5">
+        <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>44590</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>44591</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>44592</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>44593</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>44594</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>44595</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>44596</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>44597</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>44598</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>44599</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>44600</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>44601</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>44602</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>44603</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>44604</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>44605</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>44606</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>44607</v>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+    <sortCondition ref="A1:A36"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix A Bug For Deal Data!
</commit_message>
<xml_diff>
--- a/static/files/DateListNotibalityAnalyse.xlsx
+++ b/static/files/DateListNotibalityAnalyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeHiu\Desktop\Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E54E0-0AEE-4836-8176-5785BF799CB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3AF491-9BD5-4068-8423-856689477B4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,10 +323,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -470,10 +470,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$31</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -617,10 +617,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$31</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1719,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="A16:E16"/>
+      <selection activeCell="E150" sqref="A16:E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1989,269 +1989,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="3"/>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
     <sortCondition ref="A1:A31"/>

</xml_diff>

<commit_message>
add some start script for uwsgi
</commit_message>
<xml_diff>
--- a/static/files/DateListNotibalityAnalyse.xlsx
+++ b/static/files/DateListNotibalityAnalyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeHiu\Desktop\Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeHiu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3AF491-9BD5-4068-8423-856689477B4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472CE827-9B7A-4A48-A3C8-6E937E147E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,40 +47,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Python3</t>
+    <t>预估</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Arithmetic</t>
+    <t>制度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HAPPY Weekend</t>
+    <t>家人</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Foolish</t>
-  </si>
-  <si>
-    <t>Focus</t>
-  </si>
-  <si>
-    <t>Turn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Balance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>Understand</t>
+    <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -127,18 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -272,102 +245,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44572</c:v>
+                  <c:v>44593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44573</c:v>
+                  <c:v>44594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44573</c:v>
+                  <c:v>44595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44574</c:v>
+                  <c:v>44596</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44575</c:v>
+                  <c:v>44597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44576</c:v>
+                  <c:v>44598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44577</c:v>
+                  <c:v>44599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44578</c:v>
+                  <c:v>44600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44579</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44580</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44581</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44583</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44584</c:v>
+                  <c:v>44601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,102 +362,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44572</c:v>
+                  <c:v>44593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44573</c:v>
+                  <c:v>44594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44573</c:v>
+                  <c:v>44595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44574</c:v>
+                  <c:v>44596</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44575</c:v>
+                  <c:v>44597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44576</c:v>
+                  <c:v>44598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44577</c:v>
+                  <c:v>44599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44578</c:v>
+                  <c:v>44600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44579</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44580</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44581</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44583</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44584</c:v>
+                  <c:v>44601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$15</c:f>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,101 +479,71 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44572</c:v>
+                  <c:v>44593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44573</c:v>
+                  <c:v>44594</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44573</c:v>
+                  <c:v>44595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44574</c:v>
+                  <c:v>44596</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44575</c:v>
+                  <c:v>44597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44576</c:v>
+                  <c:v>44598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44577</c:v>
+                  <c:v>44599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44578</c:v>
+                  <c:v>44600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44579</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44580</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44581</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44582</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44583</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44584</c:v>
+                  <c:v>44601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$15</c:f>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00_);[Red]\(0.00\)</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1719,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E150" sqref="A16:E150"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1753,78 +1636,78 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44572</v>
+        <v>44593</v>
       </c>
       <c r="B2" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44573</v>
+        <v>44594</v>
       </c>
       <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>6</v>
-      </c>
       <c r="D3" s="2">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>44573</v>
+      <c r="A4" s="1">
+        <v>44595</v>
       </c>
       <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
-        <v>6</v>
-      </c>
       <c r="D4" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44574</v>
+        <v>44596</v>
       </c>
       <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44575</v>
+        <v>44597</v>
       </c>
       <c r="B6" s="2">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -1833,160 +1716,75 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44576</v>
+        <v>44598</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44577</v>
+        <v>44599</v>
       </c>
       <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
-        <v>7</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>44578</v>
+      <c r="A9" s="1">
+        <v>44600</v>
       </c>
       <c r="B9" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>44579</v>
+      <c r="A10" s="1">
+        <v>44601</v>
       </c>
       <c r="B10" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>44580</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2">
         <v>6</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>44581</v>
-      </c>
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
-        <v>6</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>44582</v>
-      </c>
-      <c r="B13" s="2">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2">
-        <v>6</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>44583</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>44584</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>